<commit_message>
validator: add > 0 check for ids, improve comments
</commit_message>
<xml_diff>
--- a/src/python/230/invalid_data2.xlsx
+++ b/src/python/230/invalid_data2.xlsx
@@ -685,40 +685,40 @@
   </sheetData>
   <dataValidations count="16">
     <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
       <formula1>50</formula1>
@@ -866,28 +866,28 @@
   </sheetData>
   <dataValidations count="10">
     <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
       <formula1>50</formula1>
@@ -1067,43 +1067,43 @@
   </sheetData>
   <dataValidations count="15">
     <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole" operator="greaterThanOrEqual">
       <formula1>0</formula1>
@@ -1373,37 +1373,37 @@
   </sheetData>
   <dataValidations count="16">
     <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
-    </dataValidation>
-    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
-      <formula1>=COUNTIF($A:$A, A2) = 1</formula1>
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>=(COUNTIF($A:$A, A2) = 1)AND(=$A &gt; 0)</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole" operator="greaterThanOrEqual">
       <formula1>0</formula1>

</xml_diff>